<commit_message>
Add a4 and initial code for question a), b), c)
</commit_message>
<xml_diff>
--- a/CS244N/timesheet.xlsx
+++ b/CS244N/timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\StanfordAI\CS244N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43037AC2-60C6-4816-8AE7-9F5E386A7AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B9F0BC-C3F0-466C-8CBC-DED06DE7A927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{49ECC57B-DC97-4193-A22A-014B724C54C2}"/>
+    <workbookView xWindow="38280" yWindow="2265" windowWidth="29040" windowHeight="15720" xr2:uid="{49ECC57B-DC97-4193-A22A-014B724C54C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>wk</t>
   </si>
@@ -130,23 +130,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -458,7 +451,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,78 +459,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF922A39-E683-4FA9-BACE-BA5DD720415F}">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A2:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="11" width="9.140625" style="5"/>
+    <col min="3" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
         <v>1.5</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="6">
+      <c r="I3" s="5"/>
+      <c r="J3" s="4">
         <f>SUM(C3:I3)</f>
         <v>2.5</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <f>SUM(J3:J4)</f>
         <v>10</v>
       </c>
@@ -546,46 +539,46 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
         <v>3</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <v>4.5</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="6">
+      <c r="I4" s="5"/>
+      <c r="J4" s="4">
         <f>SUM(C4:I4)</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
         <f>SUM(C6:I6)</f>
         <v>2</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <f>SUM(J6:J7)</f>
         <v>2</v>
       </c>
@@ -594,290 +587,141 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4">
         <f>SUM(C7:I7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <f>A6+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="6">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
         <f>SUM(C9:I9)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
         <f>SUM(J9:J10)</f>
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>12</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="6">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
+        <v>8</v>
+      </c>
+      <c r="H10" s="5">
+        <v>6</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4">
         <f>SUM(C10:I10)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="7"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <f>A9+1</f>
         <v>4</v>
       </c>
-      <c r="J12" s="5">
-        <f t="shared" ref="J4:J33" si="0">SUM(C12:I12)</f>
-        <v>0</v>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4">
+        <f>SUM(C12:I12)</f>
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <f>SUM(J12:J13)</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <f t="shared" ref="A13:A33" si="1">A12+1</f>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="4">
+        <f>SUM(C13:I13)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f>A12+1</f>
         <v>5</v>
       </c>
-      <c r="J13" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <f t="shared" si="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="J18" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J19" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="J20" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="J21" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="J22" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="J25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="J26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="J27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="J28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="J29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="J31" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="J32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="J33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>